<commit_message>
fix: add 32KHz crystal to BOM and change RTC package
</commit_message>
<xml_diff>
--- a/HW/BOM.xlsx
+++ b/HW/BOM.xlsx
@@ -13,8 +13,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">List1!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">List1!$A$1:$E$99</definedName>
-    <definedName name="SingleNixieClock" localSheetId="0">List1!$A$1:$AA$101</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">List1!$A$1:$E$100</definedName>
+    <definedName name="SingleNixieClock" localSheetId="0">List1!$A$1:$AA$102</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="270">
   <si>
     <t>Part</t>
   </si>
@@ -482,9 +482,6 @@
     <t>895-FT232RL</t>
   </si>
   <si>
-    <t>IO1</t>
-  </si>
-  <si>
     <t>DS1339</t>
   </si>
   <si>
@@ -906,6 +903,18 @@
   </si>
   <si>
     <t>Qty</t>
+  </si>
+  <si>
+    <t>MSOP08</t>
+  </si>
+  <si>
+    <t>IC3</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>CC5V-T1A 32.768KHz</t>
   </si>
 </sst>
 </file>
@@ -1376,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1403,7 +1412,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -1418,10 +1427,10 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" ht="14" customHeight="1" thickTop="1">
@@ -1438,7 +1447,7 @@
         <v>805</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>8</v>
@@ -1450,7 +1459,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="7" customFormat="1">
@@ -1467,7 +1476,7 @@
         <v>805</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>8</v>
@@ -1479,7 +1488,7 @@
         <v>14</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="7" customFormat="1">
@@ -1496,7 +1505,7 @@
         <v>603</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>8</v>
@@ -1508,7 +1517,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="7" customFormat="1">
@@ -1525,7 +1534,7 @@
         <v>805</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>8</v>
@@ -1537,7 +1546,7 @@
         <v>14</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1">
@@ -1554,7 +1563,7 @@
         <v>603</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>8</v>
@@ -1566,7 +1575,7 @@
         <v>18</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1">
@@ -1583,7 +1592,7 @@
         <v>805</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>8</v>
@@ -1595,7 +1604,7 @@
         <v>14</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1">
@@ -1612,7 +1621,7 @@
         <v>603</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>8</v>
@@ -1624,7 +1633,7 @@
         <v>18</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="7" customFormat="1">
@@ -1641,7 +1650,7 @@
         <v>805</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>8</v>
@@ -1653,7 +1662,7 @@
         <v>14</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="7" customFormat="1">
@@ -1670,7 +1679,7 @@
         <v>805</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>8</v>
@@ -1682,7 +1691,7 @@
         <v>10</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="7" customFormat="1">
@@ -1699,7 +1708,7 @@
         <v>805</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>8</v>
@@ -1711,7 +1720,7 @@
         <v>14</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1">
@@ -1728,7 +1737,7 @@
         <v>805</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>8</v>
@@ -1740,7 +1749,7 @@
         <v>14</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="7" customFormat="1">
@@ -1757,7 +1766,7 @@
         <v>805</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>8</v>
@@ -1769,7 +1778,7 @@
         <v>14</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="7" customFormat="1">
@@ -1786,7 +1795,7 @@
         <v>805</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>8</v>
@@ -1798,7 +1807,7 @@
         <v>14</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="7" customFormat="1">
@@ -1815,7 +1824,7 @@
         <v>805</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>8</v>
@@ -1827,7 +1836,7 @@
         <v>14</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="7" customFormat="1">
@@ -1844,7 +1853,7 @@
         <v>805</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>8</v>
@@ -1856,7 +1865,7 @@
         <v>10</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1">
@@ -1873,7 +1882,7 @@
         <v>805</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>32</v>
@@ -1885,7 +1894,7 @@
         <v>34</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1">
@@ -1902,7 +1911,7 @@
         <v>1206</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>8</v>
@@ -1911,7 +1920,7 @@
         <v>36</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I18" s="6">
         <v>2522499</v>
@@ -1931,7 +1940,7 @@
         <v>805</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>8</v>
@@ -1943,7 +1952,7 @@
         <v>14</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1">
@@ -1960,7 +1969,7 @@
         <v>805</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>8</v>
@@ -1972,7 +1981,7 @@
         <v>14</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1">
@@ -1989,19 +1998,19 @@
         <v>2420</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1">
@@ -2018,7 +2027,7 @@
         <v>603</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>8</v>
@@ -2030,7 +2039,7 @@
         <v>18</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1">
@@ -2047,19 +2056,19 @@
         <v>44</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1">
@@ -2076,7 +2085,7 @@
         <v>805</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>8</v>
@@ -2088,7 +2097,7 @@
         <v>14</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1">
@@ -2105,19 +2114,19 @@
         <v>2420</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1">
@@ -2134,19 +2143,19 @@
         <v>44</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1">
@@ -2163,7 +2172,7 @@
         <v>805</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>32</v>
@@ -2175,7 +2184,7 @@
         <v>34</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1">
@@ -2192,7 +2201,7 @@
         <v>805</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>8</v>
@@ -2204,7 +2213,7 @@
         <v>14</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1">
@@ -2221,19 +2230,19 @@
         <v>52</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1">
@@ -2250,19 +2259,19 @@
         <v>52</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="7" customFormat="1">
@@ -2279,7 +2288,7 @@
         <v>402</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>56</v>
@@ -2291,7 +2300,7 @@
         <v>58</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="7" customFormat="1">
@@ -2308,19 +2317,19 @@
         <v>44</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1">
@@ -2337,7 +2346,7 @@
         <v>1206</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>8</v>
@@ -2366,7 +2375,7 @@
         <v>1206</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>8</v>
@@ -2375,7 +2384,7 @@
         <v>36</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I34" s="6">
         <v>2522499</v>
@@ -2395,7 +2404,7 @@
         <v>1206</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>8</v>
@@ -2407,7 +2416,7 @@
         <v>67</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="7" customFormat="1">
@@ -2424,7 +2433,7 @@
         <v>1206</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>8</v>
@@ -2436,7 +2445,7 @@
         <v>67</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1">
@@ -2453,7 +2462,7 @@
         <v>1206</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>8</v>
@@ -2465,7 +2474,7 @@
         <v>67</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="7" customFormat="1">
@@ -2482,16 +2491,16 @@
         <v>72</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>71</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I38" s="6">
         <v>9551824</v>
@@ -2511,7 +2520,7 @@
         <v>75</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>76</v>
@@ -2523,7 +2532,7 @@
         <v>77</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="7" customFormat="1">
@@ -2540,7 +2549,7 @@
         <v>805</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>32</v>
@@ -2552,7 +2561,7 @@
         <v>81</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="7" customFormat="1">
@@ -2569,7 +2578,7 @@
         <v>805</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>32</v>
@@ -2581,7 +2590,7 @@
         <v>81</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1">
@@ -2598,7 +2607,7 @@
         <v>805</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>32</v>
@@ -2610,7 +2619,7 @@
         <v>81</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="7" customFormat="1" ht="14" customHeight="1">
@@ -2618,7 +2627,7 @@
         <v>84</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C43" s="6">
         <v>1</v>
@@ -2627,16 +2636,16 @@
         <v>85</v>
       </c>
       <c r="E43" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="F43" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>248</v>
-      </c>
       <c r="H43" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I43" s="6">
         <v>8806543</v>
@@ -2656,7 +2665,7 @@
         <v>88</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F44" s="8" t="s">
         <v>89</v>
@@ -2668,7 +2677,7 @@
         <v>90</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="7" customFormat="1">
@@ -2685,16 +2694,16 @@
         <v>93</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>101</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I45" s="6">
         <v>3126192</v>
@@ -2714,16 +2723,16 @@
         <v>96</v>
       </c>
       <c r="E46" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="F46" s="6" t="s">
+      <c r="G46" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="G46" s="6" t="s">
-        <v>246</v>
-      </c>
       <c r="H46" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I46" s="6">
         <v>2514157</v>
@@ -2772,7 +2781,7 @@
         <v>106</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>101</v>
@@ -2801,19 +2810,19 @@
         <v>111</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="7" customFormat="1">
@@ -2859,7 +2868,7 @@
         <v>121</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>122</v>
@@ -2876,28 +2885,28 @@
     </row>
     <row r="52" spans="1:9" s="7" customFormat="1">
       <c r="A52" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>126</v>
-      </c>
       <c r="C52" s="6">
         <v>1</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I52" s="6">
         <v>3404546</v>
@@ -2905,7 +2914,7 @@
     </row>
     <row r="53" spans="1:9" s="7" customFormat="1">
       <c r="A53" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B53" s="6">
         <v>4028</v>
@@ -2914,48 +2923,48 @@
         <v>1</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="7" customFormat="1">
       <c r="A54" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="C54" s="6">
+        <v>1</v>
+      </c>
+      <c r="D54" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="6">
-        <v>1</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>132</v>
-      </c>
       <c r="E54" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I54" s="6">
         <v>3019726</v>
@@ -2963,28 +2972,28 @@
     </row>
     <row r="55" spans="1:9" s="7" customFormat="1">
       <c r="A55" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B55" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="C55" s="6">
+        <v>1</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C55" s="6">
-        <v>1</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F55" s="6" t="s">
+      <c r="G55" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="G55" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="H55" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I55" s="6">
         <v>1688077</v>
@@ -2992,10 +3001,10 @@
     </row>
     <row r="56" spans="1:9" s="7" customFormat="1">
       <c r="A56" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B56" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>138</v>
       </c>
       <c r="C56" s="6">
         <v>1</v>
@@ -3004,16 +3013,16 @@
         <v>402</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>56</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I56" s="6">
         <v>1515368</v>
@@ -3021,10 +3030,10 @@
     </row>
     <row r="57" spans="1:9" s="7" customFormat="1">
       <c r="A57" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B57" s="6" t="s">
         <v>142</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>143</v>
       </c>
       <c r="C57" s="6">
         <v>1</v>
@@ -3033,16 +3042,16 @@
         <v>1206</v>
       </c>
       <c r="E57" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F57" s="6" t="s">
+      <c r="G57" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G57" s="6" t="s">
-        <v>146</v>
-      </c>
       <c r="H57" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I57" s="6">
         <v>2286943</v>
@@ -3050,28 +3059,28 @@
     </row>
     <row r="58" spans="1:9" s="7" customFormat="1">
       <c r="A58" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B58" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B58" s="6" t="s">
+      <c r="C58" s="6">
+        <v>1</v>
+      </c>
+      <c r="D58" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="C58" s="6">
-        <v>1</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>149</v>
-      </c>
       <c r="E58" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="F58" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="F58" s="6" t="s">
-        <v>254</v>
-      </c>
       <c r="G58" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I58" s="6">
         <v>2775426</v>
@@ -3079,10 +3088,10 @@
     </row>
     <row r="59" spans="1:9" s="7" customFormat="1">
       <c r="A59" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>151</v>
       </c>
       <c r="C59" s="6">
         <v>1</v>
@@ -3091,27 +3100,27 @@
         <v>805</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="7" customFormat="1">
       <c r="A60" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="B60" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="C60" s="6">
         <v>1</v>
@@ -3120,27 +3129,27 @@
         <v>805</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="61" spans="1:9" s="7" customFormat="1">
       <c r="A61" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C61" s="6">
         <v>1</v>
@@ -3149,85 +3158,77 @@
         <v>805</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="7" customFormat="1">
       <c r="A62" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="C62" s="6">
+        <v>1</v>
+      </c>
+      <c r="D62" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="C62" s="6">
-        <v>1</v>
-      </c>
-      <c r="D62" s="6" t="s">
+      <c r="E62" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="F62" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E62" s="6" t="s">
-        <v>239</v>
-      </c>
-      <c r="F62" s="6" t="s">
+      <c r="G62" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="G62" s="6" t="s">
+      <c r="H62" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="H62" s="6" t="s">
-        <v>161</v>
-      </c>
       <c r="I62" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="63" spans="1:9" s="7" customFormat="1">
       <c r="A63" s="6" t="s">
-        <v>162</v>
+        <v>268</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>163</v>
+        <v>269</v>
       </c>
       <c r="C63" s="6">
         <v>1</v>
       </c>
       <c r="D63" s="6">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F63" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="G63" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="H63" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I63" s="6" t="s">
-        <v>238</v>
-      </c>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
     </row>
     <row r="64" spans="1:9" s="7" customFormat="1">
       <c r="A64" s="6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C64" s="6">
         <v>1</v>
@@ -3236,257 +3237,257 @@
         <v>805</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="7" customFormat="1">
       <c r="A65" s="6" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C65" s="6">
         <v>1</v>
       </c>
       <c r="D65" s="6">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>170</v>
+        <v>237</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="I65" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="7" customFormat="1">
       <c r="A66" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C66" s="6">
         <v>1</v>
       </c>
       <c r="D66" s="6">
-        <v>805</v>
+        <v>603</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>238</v>
+        <v>168</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>238</v>
+        <v>169</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>238</v>
+        <v>170</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="7" customFormat="1">
       <c r="A67" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C67" s="6">
         <v>1</v>
       </c>
       <c r="D67" s="6">
-        <v>1206</v>
+        <v>805</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="7" customFormat="1">
       <c r="A68" s="6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C68" s="6">
         <v>1</v>
       </c>
       <c r="D68" s="6">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F68" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:9" s="7" customFormat="1">
       <c r="A69" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C69" s="6">
+        <v>1</v>
+      </c>
+      <c r="D69" s="6">
+        <v>805</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H69" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="7" customFormat="1">
+      <c r="A70" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B70" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C70" s="6">
+        <v>1</v>
+      </c>
+      <c r="D70" s="6">
+        <v>1206</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F70" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>256</v>
-      </c>
-      <c r="C69" s="6">
-        <v>1</v>
-      </c>
-      <c r="D69" s="6">
-        <v>1206</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F69" s="6" t="s">
+      <c r="G70" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="G69" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I69" s="6"/>
-    </row>
-    <row r="70" spans="1:9" s="9" customFormat="1">
-      <c r="A70" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="C70" s="8">
-        <v>1</v>
-      </c>
-      <c r="D70" s="8">
-        <v>2512</v>
-      </c>
-      <c r="E70" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="H70" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="I70" s="8" t="s">
-        <v>238</v>
-      </c>
+      <c r="H70" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" s="9" customFormat="1">
       <c r="A71" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C71" s="8">
         <v>1</v>
       </c>
       <c r="D71" s="8">
+        <v>2512</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F71" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I71" s="8" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="9" customFormat="1">
+      <c r="A72" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" s="8">
+        <v>1</v>
+      </c>
+      <c r="D72" s="8">
         <v>805</v>
       </c>
-      <c r="E71" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="I71" s="8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" s="7" customFormat="1">
-      <c r="A72" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="B72" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="C72" s="6">
-        <v>1</v>
-      </c>
-      <c r="D72" s="6">
-        <v>603</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="G72" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="H72" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I72" s="6" t="s">
-        <v>238</v>
+      <c r="E72" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H72" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I72" s="8" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="7" customFormat="1">
       <c r="A73" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C73" s="6">
         <v>1</v>
@@ -3495,83 +3496,83 @@
         <v>603</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="7" customFormat="1">
       <c r="A74" s="6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>257</v>
+        <v>185</v>
       </c>
       <c r="C74" s="6">
         <v>1</v>
       </c>
       <c r="D74" s="6">
-        <v>1206</v>
+        <v>603</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>188</v>
+        <v>237</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I74" s="6"/>
+        <v>237</v>
+      </c>
+      <c r="I74" s="6" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="75" spans="1:9" s="7" customFormat="1">
       <c r="A75" s="6" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>190</v>
+        <v>256</v>
       </c>
       <c r="C75" s="6">
         <v>1</v>
       </c>
       <c r="D75" s="6">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>238</v>
+        <v>168</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>238</v>
+        <v>187</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I75" s="6" t="s">
-        <v>238</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="I75" s="6"/>
     </row>
     <row r="76" spans="1:9" s="7" customFormat="1">
       <c r="A76" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C76" s="6">
         <v>1</v>
@@ -3580,27 +3581,27 @@
         <v>805</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="77" spans="1:9" s="7" customFormat="1">
       <c r="A77" s="6" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="C77" s="6">
         <v>1</v>
@@ -3609,27 +3610,27 @@
         <v>805</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F77" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="78" spans="1:9" s="7" customFormat="1">
       <c r="A78" s="6" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C78" s="6">
         <v>1</v>
@@ -3638,27 +3639,27 @@
         <v>805</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I78" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="79" spans="1:9" s="7" customFormat="1">
       <c r="A79" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C79" s="6">
         <v>1</v>
@@ -3667,27 +3668,27 @@
         <v>805</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="80" spans="1:9" s="7" customFormat="1">
       <c r="A80" s="6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C80" s="6">
         <v>1</v>
@@ -3696,27 +3697,27 @@
         <v>805</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F80" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I80" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="81" spans="1:9" s="7" customFormat="1">
       <c r="A81" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C81" s="6">
         <v>1</v>
@@ -3725,27 +3726,27 @@
         <v>805</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I81" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="82" spans="1:9" s="7" customFormat="1">
       <c r="A82" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C82" s="6">
         <v>1</v>
@@ -3754,27 +3755,27 @@
         <v>805</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H82" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I82" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="83" spans="1:9" s="7" customFormat="1">
       <c r="A83" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C83" s="6">
         <v>1</v>
@@ -3783,27 +3784,27 @@
         <v>805</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F83" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H83" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I83" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="7" customFormat="1">
       <c r="A84" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C84" s="6">
         <v>1</v>
@@ -3812,27 +3813,27 @@
         <v>805</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I84" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:9" s="7" customFormat="1">
       <c r="A85" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C85" s="6">
         <v>1</v>
@@ -3841,27 +3842,27 @@
         <v>805</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I85" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="86" spans="1:9" s="7" customFormat="1">
       <c r="A86" s="6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C86" s="6">
         <v>1</v>
@@ -3870,161 +3871,161 @@
         <v>805</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H86" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I86" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="87" spans="1:9" s="7" customFormat="1">
       <c r="A87" s="6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="C87" s="6">
         <v>1</v>
       </c>
       <c r="D87" s="6">
-        <v>2010</v>
+        <v>805</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I87" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="7" customFormat="1">
       <c r="A88" s="6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C88" s="6">
         <v>1</v>
       </c>
-      <c r="D88" s="6" t="s">
-        <v>207</v>
+      <c r="D88" s="6">
+        <v>2010</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="G88" s="7" t="s">
-        <v>206</v>
+        <v>237</v>
+      </c>
+      <c r="G88" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I88" s="6">
-        <v>2770035</v>
+        <v>237</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:9" s="7" customFormat="1">
       <c r="A89" s="6" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="C89" s="6">
         <v>1</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>238</v>
+        <v>208</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="H89" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I89" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="I89" s="6">
+        <v>2770035</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="7" customFormat="1">
       <c r="A90" s="6" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C90" s="6">
         <v>1</v>
       </c>
       <c r="D90" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E90" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F90" s="6" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="H90" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="I90" s="6">
-        <v>2114871</v>
+        <v>237</v>
+      </c>
+      <c r="I90" s="6" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="7" customFormat="1">
       <c r="A91" s="6" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B91" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C91" s="6">
+        <v>1</v>
+      </c>
+      <c r="D91" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C91" s="6">
-        <v>1</v>
-      </c>
-      <c r="D91" s="6" t="s">
+      <c r="E91" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E91" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F91" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G91" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G91" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H91" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I91" s="6">
         <v>2114871</v>
@@ -4032,28 +4033,28 @@
     </row>
     <row r="92" spans="1:9" s="7" customFormat="1">
       <c r="A92" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B92" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C92" s="6">
+        <v>1</v>
+      </c>
+      <c r="D92" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C92" s="6">
-        <v>1</v>
-      </c>
-      <c r="D92" s="6" t="s">
+      <c r="E92" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E92" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F92" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G92" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G92" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H92" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I92" s="6">
         <v>2114871</v>
@@ -4061,28 +4062,28 @@
     </row>
     <row r="93" spans="1:9" s="7" customFormat="1">
       <c r="A93" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B93" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C93" s="6">
+        <v>1</v>
+      </c>
+      <c r="D93" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C93" s="6">
-        <v>1</v>
-      </c>
-      <c r="D93" s="6" t="s">
+      <c r="E93" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E93" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F93" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G93" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G93" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H93" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I93" s="6">
         <v>2114871</v>
@@ -4090,28 +4091,28 @@
     </row>
     <row r="94" spans="1:9" s="7" customFormat="1">
       <c r="A94" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B94" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C94" s="6">
+        <v>1</v>
+      </c>
+      <c r="D94" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C94" s="6">
-        <v>1</v>
-      </c>
-      <c r="D94" s="6" t="s">
+      <c r="E94" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E94" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F94" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G94" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G94" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H94" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I94" s="6">
         <v>2114871</v>
@@ -4119,28 +4120,28 @@
     </row>
     <row r="95" spans="1:9" s="7" customFormat="1">
       <c r="A95" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B95" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C95" s="6">
+        <v>1</v>
+      </c>
+      <c r="D95" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C95" s="6">
-        <v>1</v>
-      </c>
-      <c r="D95" s="6" t="s">
+      <c r="E95" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E95" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F95" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G95" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G95" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H95" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I95" s="6">
         <v>2114871</v>
@@ -4148,28 +4149,28 @@
     </row>
     <row r="96" spans="1:9" s="7" customFormat="1">
       <c r="A96" s="6" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B96" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C96" s="6">
+        <v>1</v>
+      </c>
+      <c r="D96" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C96" s="6">
-        <v>1</v>
-      </c>
-      <c r="D96" s="6" t="s">
+      <c r="E96" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E96" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F96" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G96" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G96" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H96" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I96" s="6">
         <v>2114871</v>
@@ -4177,28 +4178,28 @@
     </row>
     <row r="97" spans="1:9" s="7" customFormat="1">
       <c r="A97" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B97" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C97" s="6">
+        <v>1</v>
+      </c>
+      <c r="D97" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C97" s="6">
-        <v>1</v>
-      </c>
-      <c r="D97" s="6" t="s">
+      <c r="E97" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E97" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F97" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G97" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G97" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H97" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I97" s="6">
         <v>2114871</v>
@@ -4206,28 +4207,28 @@
     </row>
     <row r="98" spans="1:9" s="7" customFormat="1">
       <c r="A98" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B98" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C98" s="6">
+        <v>1</v>
+      </c>
+      <c r="D98" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C98" s="6">
-        <v>1</v>
-      </c>
-      <c r="D98" s="6" t="s">
+      <c r="E98" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E98" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F98" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G98" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G98" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H98" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I98" s="6">
         <v>2114871</v>
@@ -4235,122 +4236,151 @@
     </row>
     <row r="99" spans="1:9" s="7" customFormat="1">
       <c r="A99" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B99" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C99" s="6">
+        <v>1</v>
+      </c>
+      <c r="D99" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="C99" s="6">
-        <v>1</v>
-      </c>
-      <c r="D99" s="6" t="s">
+      <c r="E99" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="E99" s="6" t="s">
-        <v>216</v>
-      </c>
       <c r="F99" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G99" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G99" s="6" t="s">
-        <v>260</v>
-      </c>
       <c r="H99" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I99" s="6">
         <v>2114871</v>
       </c>
     </row>
-    <row r="100" spans="1:9" s="3" customFormat="1" hidden="1">
-      <c r="A100" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="F100" s="2" t="s">
+    <row r="100" spans="1:9" s="7" customFormat="1">
+      <c r="A100" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C100" s="6">
+        <v>1</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F100" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="G100" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="H100" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="I100" s="2">
+      <c r="G100" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="H100" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I100" s="6">
+        <v>2114871</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" s="3" customFormat="1" hidden="1">
+      <c r="A101" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I101" s="2">
         <v>149319</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="5" customFormat="1" hidden="1">
-      <c r="A101" s="4" t="s">
+    <row r="102" spans="1:9" s="5" customFormat="1" hidden="1">
+      <c r="A102" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B102" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B101" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="C101" s="4"/>
-      <c r="D101" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="E101" s="4" t="s">
+      <c r="C102" s="4"/>
+      <c r="D102" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F102" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="F101" s="4" t="s">
+      <c r="G102" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="G101" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="H101" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="I101" s="4" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9">
-      <c r="A102" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="B102" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="C102" s="14">
-        <v>1</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>235</v>
+      <c r="H102" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I102" s="4" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" s="14" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="B103" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C103" s="14">
+        <v>1</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B104" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C104" s="14">
+        <v>11</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E104" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="C103" s="14">
-        <v>11</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="15" customHeight="1"/>
+    </row>
+    <row r="111" spans="1:9" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: add el cap to HV output
</commit_message>
<xml_diff>
--- a/HW/BOM.xlsx
+++ b/HW/BOM.xlsx
@@ -13,8 +13,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">List1!$1:$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">List1!$A$1:$E$100</definedName>
-    <definedName name="SingleNixieClock" localSheetId="0">List1!$A$1:$AA$102</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">List1!$A$1:$E$101</definedName>
+    <definedName name="SingleNixieClock" localSheetId="0">List1!$A$1:$AA$103</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="273">
   <si>
     <t>Part</t>
   </si>
@@ -915,6 +915,15 @@
   </si>
   <si>
     <t>CC5V-T1A 32.768KHz</t>
+  </si>
+  <si>
+    <t>C32</t>
+  </si>
+  <si>
+    <t>4u7/250V</t>
+  </si>
+  <si>
+    <t>C_EL_3,5</t>
   </si>
 </sst>
 </file>
@@ -1385,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2334,39 +2343,31 @@
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1">
       <c r="A33" s="6" t="s">
-        <v>60</v>
+        <v>270</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>61</v>
+        <v>271</v>
       </c>
       <c r="C33" s="6">
         <v>1</v>
       </c>
-      <c r="D33" s="6">
-        <v>1206</v>
+      <c r="D33" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I33" s="6">
-        <v>2070500</v>
-      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
     </row>
     <row r="34" spans="1:9" s="7" customFormat="1">
       <c r="A34" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="C34" s="6">
         <v>1</v>
@@ -2381,21 +2382,21 @@
         <v>8</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>237</v>
+        <v>63</v>
       </c>
       <c r="I34" s="6">
-        <v>2522499</v>
+        <v>2070500</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="7" customFormat="1">
       <c r="A35" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C35" s="6">
         <v>1</v>
@@ -2410,18 +2411,18 @@
         <v>8</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="I35" s="6" t="s">
-        <v>237</v>
+        <v>237</v>
+      </c>
+      <c r="I35" s="6">
+        <v>2522499</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="7" customFormat="1">
       <c r="A36" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>43</v>
@@ -2450,7 +2451,7 @@
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1">
       <c r="A37" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>43</v>
@@ -2479,86 +2480,86 @@
     </row>
     <row r="38" spans="1:9" s="7" customFormat="1">
       <c r="A38" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>71</v>
+        <v>43</v>
       </c>
       <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="6" t="s">
-        <v>72</v>
+      <c r="D38" s="6">
+        <v>1206</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>177</v>
+        <v>8</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I38" s="6">
-        <v>9551824</v>
+        <v>67</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="7" customFormat="1">
       <c r="A39" s="6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C39" s="6">
         <v>1</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>231</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>237</v>
+        <v>237</v>
+      </c>
+      <c r="I39" s="6">
+        <v>9551824</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="7" customFormat="1">
       <c r="A40" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C40" s="6">
         <v>1</v>
       </c>
-      <c r="D40" s="6">
-        <v>805</v>
+      <c r="D40" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>237</v>
@@ -2566,7 +2567,7 @@
     </row>
     <row r="41" spans="1:9" s="7" customFormat="1">
       <c r="A41" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>79</v>
@@ -2595,7 +2596,7 @@
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1">
       <c r="A42" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>79</v>
@@ -2622,505 +2623,505 @@
         <v>237</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" ht="14" customHeight="1">
+    <row r="43" spans="1:9" s="7" customFormat="1">
       <c r="A43" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="6">
+        <v>1</v>
+      </c>
+      <c r="D43" s="6">
+        <v>805</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="7" customFormat="1" ht="14" customHeight="1">
+      <c r="A44" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="C43" s="6">
-        <v>1</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="B44" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C44" s="6">
+        <v>1</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E43" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="F43" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G44" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I43" s="6">
+      <c r="H44" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I44" s="6">
         <v>8806543</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="9" customFormat="1">
-      <c r="A44" s="8" t="s">
+    <row r="45" spans="1:9" s="9" customFormat="1">
+      <c r="A45" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B45" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="8">
-        <v>1</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="C45" s="8">
+        <v>1</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E44" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="F44" s="8" t="s">
+      <c r="F45" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G44" s="8" t="s">
+      <c r="G45" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="H44" s="8" t="s">
+      <c r="H45" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="I44" s="8" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="7" customFormat="1">
-      <c r="A45" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="6">
-        <v>1</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>249</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I45" s="6">
-        <v>3126192</v>
+      <c r="I45" s="8" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="7" customFormat="1">
       <c r="A46" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C46" s="6">
         <v>1</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>244</v>
+        <v>101</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>237</v>
       </c>
       <c r="I46" s="6">
-        <v>2514157</v>
+        <v>3126192</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="7" customFormat="1">
       <c r="A47" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C47" s="6">
         <v>1</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>100</v>
+        <v>243</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>101</v>
+        <v>244</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>102</v>
+        <v>245</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>103</v>
+        <v>237</v>
       </c>
       <c r="I47" s="6">
-        <v>3124063</v>
+        <v>2514157</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="7" customFormat="1">
       <c r="A48" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C48" s="6">
         <v>1</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>101</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="I48" s="6">
-        <v>3116503</v>
+        <v>3124063</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="7" customFormat="1">
       <c r="A49" s="6" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C49" s="6">
         <v>1</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>237</v>
+        <v>101</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>237</v>
+        <v>107</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I49" s="6" t="s">
-        <v>237</v>
+        <v>108</v>
+      </c>
+      <c r="I49" s="6">
+        <v>3116503</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="7" customFormat="1">
       <c r="A50" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C50" s="6">
         <v>1</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>115</v>
+        <v>251</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>116</v>
+        <v>237</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>117</v>
+        <v>237</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="I50" s="6">
-        <v>1439380</v>
+        <v>237</v>
+      </c>
+      <c r="I50" s="6" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="7" customFormat="1">
       <c r="A51" s="6" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="C51" s="6">
         <v>1</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>241</v>
+        <v>115</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="I51" s="6">
-        <v>1146032</v>
+        <v>1439380</v>
       </c>
     </row>
     <row r="52" spans="1:9" s="7" customFormat="1">
       <c r="A52" s="6" t="s">
-        <v>267</v>
+        <v>119</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C52" s="6">
         <v>1</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>266</v>
+        <v>121</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>244</v>
+        <v>122</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>260</v>
+        <v>123</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>237</v>
+        <v>124</v>
       </c>
       <c r="I52" s="6">
-        <v>3404546</v>
+        <v>1146032</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="7" customFormat="1">
       <c r="A53" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B53" s="6">
-        <v>4028</v>
+        <v>267</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="C53" s="6">
         <v>1</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>126</v>
+        <v>266</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>128</v>
+        <v>242</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="H53" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I53" s="6" t="s">
-        <v>237</v>
+      <c r="I53" s="6">
+        <v>3404546</v>
       </c>
     </row>
     <row r="54" spans="1:9" s="7" customFormat="1">
       <c r="A54" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
+      </c>
+      <c r="B54" s="6">
+        <v>4028</v>
       </c>
       <c r="C54" s="6">
         <v>1</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>228</v>
+        <v>128</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>134</v>
+        <v>237</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>130</v>
+        <v>237</v>
       </c>
       <c r="H54" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I54" s="6">
-        <v>3019726</v>
+      <c r="I54" s="6" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:9" s="7" customFormat="1">
       <c r="A55" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C55" s="6">
         <v>1</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>134</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>237</v>
       </c>
       <c r="I55" s="6">
-        <v>1688077</v>
+        <v>3019726</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="7" customFormat="1">
       <c r="A56" s="6" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C56" s="6">
         <v>1</v>
       </c>
-      <c r="D56" s="6">
-        <v>402</v>
+      <c r="D56" s="6" t="s">
+        <v>133</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>139</v>
+        <v>240</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>140</v>
+        <v>237</v>
       </c>
       <c r="I56" s="6">
-        <v>1515368</v>
+        <v>1688077</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="7" customFormat="1">
       <c r="A57" s="6" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C57" s="6">
         <v>1</v>
       </c>
       <c r="D57" s="6">
-        <v>1206</v>
+        <v>402</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>144</v>
+        <v>56</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>237</v>
+        <v>140</v>
       </c>
       <c r="I57" s="6">
-        <v>2286943</v>
+        <v>1515368</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="7" customFormat="1">
       <c r="A58" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C58" s="6">
         <v>1</v>
       </c>
-      <c r="D58" s="6" t="s">
-        <v>148</v>
+      <c r="D58" s="6">
+        <v>1206</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>252</v>
+        <v>143</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>253</v>
+        <v>144</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H58" s="6" t="s">
         <v>237</v>
       </c>
       <c r="I58" s="6">
-        <v>2775426</v>
+        <v>2286943</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="7" customFormat="1">
       <c r="A59" s="6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C59" s="6">
         <v>1</v>
       </c>
-      <c r="D59" s="6">
-        <v>805</v>
+      <c r="D59" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>237</v>
+        <v>147</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I59" s="6" t="s">
-        <v>237</v>
+      <c r="I59" s="6">
+        <v>2775426</v>
       </c>
     </row>
     <row r="60" spans="1:9" s="7" customFormat="1">
       <c r="A60" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C60" s="6">
         <v>1</v>
@@ -3129,7 +3130,7 @@
         <v>805</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>153</v>
+        <v>239</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>237</v>
@@ -3146,7 +3147,7 @@
     </row>
     <row r="61" spans="1:9" s="7" customFormat="1">
       <c r="A61" s="6" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>152</v>
@@ -3175,28 +3176,28 @@
     </row>
     <row r="62" spans="1:9" s="7" customFormat="1">
       <c r="A62" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C62" s="6">
         <v>1</v>
       </c>
-      <c r="D62" s="6" t="s">
-        <v>157</v>
+      <c r="D62" s="6">
+        <v>805</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>238</v>
+        <v>153</v>
       </c>
       <c r="F62" s="6" t="s">
-        <v>158</v>
+        <v>237</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>159</v>
+        <v>237</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>160</v>
+        <v>237</v>
       </c>
       <c r="I62" s="6" t="s">
         <v>237</v>
@@ -3204,60 +3205,60 @@
     </row>
     <row r="63" spans="1:9" s="7" customFormat="1">
       <c r="A63" s="6" t="s">
-        <v>268</v>
+        <v>155</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>269</v>
+        <v>156</v>
       </c>
       <c r="C63" s="6">
         <v>1</v>
       </c>
-      <c r="D63" s="6">
-        <v>1206</v>
+      <c r="D63" s="6" t="s">
+        <v>157</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6"/>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
+      <c r="F63" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="64" spans="1:9" s="7" customFormat="1">
       <c r="A64" s="6" t="s">
-        <v>161</v>
+        <v>268</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>162</v>
+        <v>269</v>
       </c>
       <c r="C64" s="6">
         <v>1</v>
       </c>
       <c r="D64" s="6">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="G64" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="H64" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I64" s="6" t="s">
-        <v>237</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
     </row>
     <row r="65" spans="1:9" s="7" customFormat="1">
       <c r="A65" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C65" s="6">
         <v>1</v>
@@ -3283,28 +3284,28 @@
     </row>
     <row r="66" spans="1:9" s="7" customFormat="1">
       <c r="A66" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C66" s="6">
         <v>1</v>
       </c>
       <c r="D66" s="6">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>163</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>168</v>
+        <v>237</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>169</v>
+        <v>237</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>170</v>
+        <v>237</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>237</v>
@@ -3312,28 +3313,28 @@
     </row>
     <row r="67" spans="1:9" s="7" customFormat="1">
       <c r="A67" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C67" s="6">
         <v>1</v>
       </c>
       <c r="D67" s="6">
-        <v>805</v>
+        <v>603</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>163</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>237</v>
+        <v>168</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>237</v>
+        <v>169</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>237</v>
+        <v>170</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>237</v>
@@ -3341,16 +3342,16 @@
     </row>
     <row r="68" spans="1:9" s="7" customFormat="1">
       <c r="A68" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C68" s="6">
         <v>1</v>
       </c>
       <c r="D68" s="6">
-        <v>1206</v>
+        <v>805</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>163</v>
@@ -3370,16 +3371,16 @@
     </row>
     <row r="69" spans="1:9" s="7" customFormat="1">
       <c r="A69" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C69" s="6">
         <v>1</v>
       </c>
       <c r="D69" s="6">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="E69" s="6" t="s">
         <v>163</v>
@@ -3399,72 +3400,72 @@
     </row>
     <row r="70" spans="1:9" s="7" customFormat="1">
       <c r="A70" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>255</v>
+        <v>175</v>
       </c>
       <c r="C70" s="6">
         <v>1</v>
       </c>
       <c r="D70" s="6">
-        <v>1206</v>
+        <v>805</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>163</v>
       </c>
       <c r="F70" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="H70" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="7" customFormat="1">
+      <c r="A71" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="C71" s="6">
+        <v>1</v>
+      </c>
+      <c r="D71" s="6">
+        <v>1206</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="G70" s="6" t="s">
+      <c r="G71" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="H70" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I70" s="6"/>
-    </row>
-    <row r="71" spans="1:9" s="9" customFormat="1">
-      <c r="A71" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="B71" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C71" s="8">
-        <v>1</v>
-      </c>
-      <c r="D71" s="8">
-        <v>2512</v>
-      </c>
-      <c r="E71" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="F71" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="I71" s="8" t="s">
-        <v>237</v>
-      </c>
+      <c r="H71" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I71" s="6"/>
     </row>
     <row r="72" spans="1:9" s="9" customFormat="1">
       <c r="A72" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C72" s="8">
         <v>1</v>
       </c>
       <c r="D72" s="8">
-        <v>805</v>
+        <v>2512</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>163</v>
@@ -3482,41 +3483,41 @@
         <v>237</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="7" customFormat="1">
-      <c r="A73" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B73" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="C73" s="6">
-        <v>1</v>
-      </c>
-      <c r="D73" s="6">
-        <v>603</v>
-      </c>
-      <c r="E73" s="6" t="s">
+    <row r="73" spans="1:9" s="9" customFormat="1">
+      <c r="A73" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C73" s="8">
+        <v>1</v>
+      </c>
+      <c r="D73" s="8">
+        <v>805</v>
+      </c>
+      <c r="E73" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="F73" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="H73" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="I73" s="6" t="s">
+      <c r="F73" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="I73" s="8" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="74" spans="1:9" s="7" customFormat="1">
       <c r="A74" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C74" s="6">
         <v>1</v>
@@ -3542,66 +3543,66 @@
     </row>
     <row r="75" spans="1:9" s="7" customFormat="1">
       <c r="A75" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>256</v>
+        <v>185</v>
       </c>
       <c r="C75" s="6">
         <v>1</v>
       </c>
       <c r="D75" s="6">
-        <v>1206</v>
+        <v>603</v>
       </c>
       <c r="E75" s="6" t="s">
         <v>163</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>168</v>
+        <v>237</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>187</v>
+        <v>237</v>
       </c>
       <c r="H75" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I75" s="6"/>
+      <c r="I75" s="6" t="s">
+        <v>237</v>
+      </c>
     </row>
     <row r="76" spans="1:9" s="7" customFormat="1">
       <c r="A76" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>189</v>
+        <v>256</v>
       </c>
       <c r="C76" s="6">
         <v>1</v>
       </c>
       <c r="D76" s="6">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>163</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>237</v>
+        <v>168</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I76" s="6" t="s">
-        <v>237</v>
-      </c>
+      <c r="I76" s="6"/>
     </row>
     <row r="77" spans="1:9" s="7" customFormat="1">
       <c r="A77" s="6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C77" s="6">
         <v>1</v>
@@ -3627,10 +3628,10 @@
     </row>
     <row r="78" spans="1:9" s="7" customFormat="1">
       <c r="A78" s="6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="C78" s="6">
         <v>1</v>
@@ -3656,7 +3657,7 @@
     </row>
     <row r="79" spans="1:9" s="7" customFormat="1">
       <c r="A79" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>175</v>
@@ -3685,7 +3686,7 @@
     </row>
     <row r="80" spans="1:9" s="7" customFormat="1">
       <c r="A80" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>175</v>
@@ -3714,7 +3715,7 @@
     </row>
     <row r="81" spans="1:9" s="7" customFormat="1">
       <c r="A81" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>175</v>
@@ -3743,7 +3744,7 @@
     </row>
     <row r="82" spans="1:9" s="7" customFormat="1">
       <c r="A82" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>175</v>
@@ -3772,7 +3773,7 @@
     </row>
     <row r="83" spans="1:9" s="7" customFormat="1">
       <c r="A83" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>175</v>
@@ -3801,7 +3802,7 @@
     </row>
     <row r="84" spans="1:9" s="7" customFormat="1">
       <c r="A84" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>175</v>
@@ -3830,7 +3831,7 @@
     </row>
     <row r="85" spans="1:9" s="7" customFormat="1">
       <c r="A85" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B85" s="6" t="s">
         <v>175</v>
@@ -3859,7 +3860,7 @@
     </row>
     <row r="86" spans="1:9" s="7" customFormat="1">
       <c r="A86" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>175</v>
@@ -3888,7 +3889,7 @@
     </row>
     <row r="87" spans="1:9" s="7" customFormat="1">
       <c r="A87" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>175</v>
@@ -3917,16 +3918,16 @@
     </row>
     <row r="88" spans="1:9" s="7" customFormat="1">
       <c r="A88" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="C88" s="6">
         <v>1</v>
       </c>
       <c r="D88" s="6">
-        <v>2010</v>
+        <v>805</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>163</v>
@@ -3946,94 +3947,94 @@
     </row>
     <row r="89" spans="1:9" s="7" customFormat="1">
       <c r="A89" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C89" s="6">
         <v>1</v>
       </c>
-      <c r="D89" s="6" t="s">
-        <v>206</v>
+      <c r="D89" s="6">
+        <v>2010</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="G89" s="7" t="s">
-        <v>205</v>
+        <v>237</v>
+      </c>
+      <c r="G89" s="6" t="s">
+        <v>237</v>
       </c>
       <c r="H89" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I89" s="6">
-        <v>2770035</v>
+      <c r="I89" s="6" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="90" spans="1:9" s="7" customFormat="1">
       <c r="A90" s="6" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C90" s="6">
         <v>1</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="G90" s="6" t="s">
-        <v>237</v>
+        <v>208</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>205</v>
       </c>
       <c r="H90" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I90" s="6" t="s">
-        <v>237</v>
+      <c r="I90" s="6">
+        <v>2770035</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="7" customFormat="1">
       <c r="A91" s="6" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C91" s="6">
         <v>1</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E91" s="6" t="s">
         <v>215</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="H91" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="I91" s="6">
-        <v>2114871</v>
+      <c r="I91" s="6" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="92" spans="1:9" s="7" customFormat="1">
       <c r="A92" s="6" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>213</v>
@@ -4062,7 +4063,7 @@
     </row>
     <row r="93" spans="1:9" s="7" customFormat="1">
       <c r="A93" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>213</v>
@@ -4091,7 +4092,7 @@
     </row>
     <row r="94" spans="1:9" s="7" customFormat="1">
       <c r="A94" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>213</v>
@@ -4120,7 +4121,7 @@
     </row>
     <row r="95" spans="1:9" s="7" customFormat="1">
       <c r="A95" s="6" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>213</v>
@@ -4149,7 +4150,7 @@
     </row>
     <row r="96" spans="1:9" s="7" customFormat="1">
       <c r="A96" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>213</v>
@@ -4178,7 +4179,7 @@
     </row>
     <row r="97" spans="1:9" s="7" customFormat="1">
       <c r="A97" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>213</v>
@@ -4207,7 +4208,7 @@
     </row>
     <row r="98" spans="1:9" s="7" customFormat="1">
       <c r="A98" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>213</v>
@@ -4236,7 +4237,7 @@
     </row>
     <row r="99" spans="1:9" s="7" customFormat="1">
       <c r="A99" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>213</v>
@@ -4265,7 +4266,7 @@
     </row>
     <row r="100" spans="1:9" s="7" customFormat="1">
       <c r="A100" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>213</v>
@@ -4292,95 +4293,124 @@
         <v>2114871</v>
       </c>
     </row>
-    <row r="101" spans="1:9" s="3" customFormat="1" hidden="1">
-      <c r="A101" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B101" s="2" t="s">
+    <row r="101" spans="1:9" s="7" customFormat="1">
+      <c r="A101" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C101" s="6">
+        <v>1</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="G101" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="H101" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="I101" s="6">
+        <v>2114871</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" s="3" customFormat="1" hidden="1">
+      <c r="A102" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="E101" s="2" t="s">
+      <c r="C102" s="2"/>
+      <c r="D102" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="F101" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="G101" s="2" t="s">
+      <c r="G102" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="H101" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="I101" s="2">
+      <c r="H102" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="I102" s="2">
         <v>149319</v>
       </c>
     </row>
-    <row r="102" spans="1:9" s="5" customFormat="1" hidden="1">
-      <c r="A102" s="4" t="s">
+    <row r="103" spans="1:9" s="5" customFormat="1" hidden="1">
+      <c r="A103" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4" t="s">
+      <c r="C103" s="4"/>
+      <c r="D103" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E102" s="4" t="s">
+      <c r="E103" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="F102" s="4" t="s">
+      <c r="F103" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="G102" s="4" t="s">
+      <c r="G103" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="H102" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="I102" s="4" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9">
-      <c r="A103" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="B103" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="C103" s="14">
-        <v>1</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>234</v>
+      <c r="H103" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="I103" s="4" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" s="14" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="B104" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C104" s="14">
+        <v>1</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="B105" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="C104" s="14">
+      <c r="C105" s="14">
         <v>11</v>
       </c>
-      <c r="D104" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E104" s="6" t="s">
+      <c r="D105" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E105" s="6" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="15" customHeight="1"/>
+    <row r="112" spans="1:9" ht="15" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>